<commit_message>
TestNG package created 26-July
</commit_message>
<xml_diff>
--- a/ExcelSheets/TestData_Read.xlsx
+++ b/ExcelSheets/TestData_Read.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
     <sheet name="test" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="url" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>First Name</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>url</t>
   </si>
 </sst>
 </file>
@@ -539,7 +542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -557,12 +560,95 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>